<commit_message>
Changed CHX_adapted to Adapted Updated Theme
</commit_message>
<xml_diff>
--- a/Data/metadata.xlsx
+++ b/Data/metadata.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">73_A_125</t>
   </si>
   <si>
-    <t xml:space="preserve">CHX_Adapted</t>
+    <t xml:space="preserve">Adapted</t>
   </si>
   <si>
     <t xml:space="preserve">73_A</t>
@@ -515,7 +515,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1488,44 +1488,28 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0"/>
-      <c r="F38" s="0"/>
-      <c r="G38" s="0"/>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0"/>
-      <c r="F39" s="0"/>
-      <c r="G39" s="0"/>
+      <c r="G39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0"/>
-      <c r="F40" s="0"/>
-      <c r="G40" s="0"/>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0"/>
-      <c r="F42" s="0"/>
-      <c r="G42" s="0"/>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0"/>
-      <c r="F43" s="0"/>
-      <c r="G43" s="0"/>
+      <c r="G43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0"/>
-      <c r="F44" s="0"/>
-      <c r="G44" s="0"/>
+      <c r="G44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0"/>
-      <c r="F45" s="0"/>
-      <c r="G45" s="0"/>
+      <c r="G45" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>